<commit_message>
Expression construct selection: excluded SGC Oxford plasmids which are not designed for E coli expression.
</commit_message>
<xml_diff>
--- a/plasmids/SGC/Oxford_SGC_Clones/oxford sgc clones for sbs_020513.xlsx
+++ b/plasmids/SGC/Oxford_SGC_Clones/oxford sgc clones for sbs_020513.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14385" yWindow="525" windowWidth="14460" windowHeight="11640"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28280"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7913" uniqueCount="3946">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7914" uniqueCount="3946">
   <si>
     <t>Protein Family</t>
   </si>
@@ -11858,8 +11863,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="19">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -12037,25 +12042,25 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -12063,39 +12068,39 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -12323,8 +12328,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -12337,7 +12341,8 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Bad" xfId="8" builtinId="27"/>
@@ -12749,33 +12754,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD499"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A479" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G503" sqref="G503"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A337" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J353" sqref="J353"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="1"/>
-    <col min="2" max="2" width="12.5703125" style="1" customWidth="1"/>
-    <col min="3" max="4" width="18.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" style="1" customWidth="1"/>
-    <col min="6" max="8" width="15.42578125" style="1"/>
-    <col min="9" max="9" width="30.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5" style="1"/>
+    <col min="2" max="2" width="12.5" style="1" customWidth="1"/>
+    <col min="3" max="4" width="18.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" style="1" customWidth="1"/>
+    <col min="6" max="8" width="15.5" style="1"/>
+    <col min="9" max="9" width="30.83203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="23.5" style="1" customWidth="1"/>
     <col min="11" max="11" width="25" style="1" customWidth="1"/>
-    <col min="12" max="17" width="15.42578125" style="1"/>
-    <col min="18" max="18" width="24.42578125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="40.85546875" style="1" customWidth="1"/>
+    <col min="12" max="17" width="15.5" style="1"/>
+    <col min="18" max="18" width="24.5" style="1" customWidth="1"/>
+    <col min="19" max="19" width="40.83203125" style="1" customWidth="1"/>
     <col min="20" max="20" width="41" style="1" customWidth="1"/>
-    <col min="21" max="21" width="37.42578125" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="15.42578125" style="1"/>
+    <col min="21" max="21" width="37.5" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="15.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="85" customFormat="1" ht="45">
+    <row r="1" spans="1:29" s="85" customFormat="1" ht="28">
       <c r="A1" s="81" t="s">
         <v>3292</v>
       </c>
@@ -12864,7 +12869,7 @@
         <v>2706</v>
       </c>
     </row>
-    <row r="2" spans="1:29" s="3" customFormat="1" ht="18.75">
+    <row r="2" spans="1:29" s="3" customFormat="1" ht="18">
       <c r="A2" s="26" t="s">
         <v>2793</v>
       </c>
@@ -19647,7 +19652,7 @@
       <c r="AB98" s="24"/>
       <c r="AC98" s="24"/>
     </row>
-    <row r="99" spans="1:29" s="3" customFormat="1" ht="18.75">
+    <row r="99" spans="1:29" s="3" customFormat="1" ht="18">
       <c r="A99" s="26" t="s">
         <v>2794</v>
       </c>
@@ -26442,7 +26447,7 @@
       <c r="AB195" s="24"/>
       <c r="AC195" s="24"/>
     </row>
-    <row r="196" spans="1:29" s="3" customFormat="1" ht="18.75">
+    <row r="196" spans="1:29" s="3" customFormat="1" ht="18">
       <c r="A196" s="26" t="s">
         <v>2795</v>
       </c>
@@ -33285,7 +33290,7 @@
       <c r="AB292" s="24"/>
       <c r="AC292" s="24"/>
     </row>
-    <row r="293" spans="1:29" s="3" customFormat="1" ht="18.75">
+    <row r="293" spans="1:29" s="3" customFormat="1" ht="18">
       <c r="A293" s="26" t="s">
         <v>2796</v>
       </c>
@@ -37407,7 +37412,9 @@
       <c r="I352" s="49" t="s">
         <v>3881</v>
       </c>
-      <c r="J352" s="116"/>
+      <c r="J352" s="116" t="s">
+        <v>1637</v>
+      </c>
       <c r="K352" s="116" t="s">
         <v>1639</v>
       </c>
@@ -38843,7 +38850,7 @@
       <c r="AB389" s="4"/>
       <c r="AC389" s="4"/>
     </row>
-    <row r="390" spans="1:29" s="3" customFormat="1" ht="18.75">
+    <row r="390" spans="1:29" s="3" customFormat="1" ht="18">
       <c r="A390" s="26" t="s">
         <v>2797</v>
       </c>
@@ -44856,7 +44863,7 @@
       <c r="AA488" s="112"/>
       <c r="AB488" s="104"/>
       <c r="AC488" s="104"/>
-      <c r="AD488" s="154"/>
+      <c r="AD488" s="144"/>
     </row>
     <row r="489" spans="1:30">
       <c r="A489" s="104" t="s">
@@ -44933,50 +44940,50 @@
       <c r="AA489" s="116"/>
       <c r="AB489" s="116"/>
       <c r="AC489" s="116"/>
-      <c r="AD489" s="154"/>
+      <c r="AD489" s="144"/>
     </row>
     <row r="490" spans="1:30">
-      <c r="A490" s="150" t="s">
+      <c r="A490" s="149" t="s">
         <v>3407</v>
       </c>
-      <c r="B490" s="146" t="s">
+      <c r="B490" s="145" t="s">
         <v>2709</v>
       </c>
-      <c r="C490" s="148" t="s">
+      <c r="C490" s="147" t="s">
         <v>3607</v>
       </c>
-      <c r="D490" s="146"/>
-      <c r="E490" s="146" t="s">
+      <c r="D490" s="145"/>
+      <c r="E490" s="145" t="s">
         <v>3608</v>
       </c>
-      <c r="F490" s="146" t="s">
+      <c r="F490" s="145" t="s">
         <v>3609</v>
       </c>
-      <c r="G490" s="146" t="s">
+      <c r="G490" s="145" t="s">
         <v>270</v>
       </c>
-      <c r="H490" s="146" t="s">
+      <c r="H490" s="145" t="s">
         <v>3613</v>
       </c>
-      <c r="I490" s="152"/>
-      <c r="J490" s="146" t="s">
+      <c r="I490" s="151"/>
+      <c r="J490" s="145" t="s">
         <v>1637</v>
       </c>
-      <c r="K490" s="146"/>
-      <c r="L490" s="146"/>
-      <c r="M490" s="144" t="s">
+      <c r="K490" s="145"/>
+      <c r="L490" s="145"/>
+      <c r="M490" s="153" t="s">
         <v>3862</v>
       </c>
-      <c r="N490" s="146" t="s">
+      <c r="N490" s="145" t="s">
         <v>3610</v>
       </c>
-      <c r="O490" s="146" t="s">
+      <c r="O490" s="145" t="s">
         <v>3477</v>
       </c>
-      <c r="P490" s="146"/>
-      <c r="Q490" s="146"/>
-      <c r="R490" s="146"/>
-      <c r="S490" s="146"/>
+      <c r="P490" s="145"/>
+      <c r="Q490" s="145"/>
+      <c r="R490" s="145"/>
+      <c r="S490" s="145"/>
       <c r="T490" s="116" t="s">
         <v>3875</v>
       </c>
@@ -45005,25 +45012,25 @@
       <c r="AC490" s="116"/>
     </row>
     <row r="491" spans="1:30">
-      <c r="A491" s="151"/>
-      <c r="B491" s="147"/>
-      <c r="C491" s="149"/>
-      <c r="D491" s="147"/>
-      <c r="E491" s="147"/>
-      <c r="F491" s="147"/>
-      <c r="G491" s="147"/>
-      <c r="H491" s="147"/>
-      <c r="I491" s="153"/>
-      <c r="J491" s="147"/>
-      <c r="K491" s="147"/>
-      <c r="L491" s="147"/>
-      <c r="M491" s="145"/>
-      <c r="N491" s="147"/>
-      <c r="O491" s="147"/>
-      <c r="P491" s="147"/>
-      <c r="Q491" s="147"/>
-      <c r="R491" s="147"/>
-      <c r="S491" s="147"/>
+      <c r="A491" s="150"/>
+      <c r="B491" s="146"/>
+      <c r="C491" s="148"/>
+      <c r="D491" s="146"/>
+      <c r="E491" s="146"/>
+      <c r="F491" s="146"/>
+      <c r="G491" s="146"/>
+      <c r="H491" s="146"/>
+      <c r="I491" s="152"/>
+      <c r="J491" s="146"/>
+      <c r="K491" s="146"/>
+      <c r="L491" s="146"/>
+      <c r="M491" s="154"/>
+      <c r="N491" s="146"/>
+      <c r="O491" s="146"/>
+      <c r="P491" s="146"/>
+      <c r="Q491" s="146"/>
+      <c r="R491" s="146"/>
+      <c r="S491" s="146"/>
       <c r="T491" s="116" t="s">
         <v>3611</v>
       </c>
@@ -45186,6 +45193,15 @@
     <sortCondition ref="B2:B3"/>
   </sortState>
   <mergeCells count="19">
+    <mergeCell ref="M490:M491"/>
+    <mergeCell ref="L490:L491"/>
+    <mergeCell ref="K490:K491"/>
+    <mergeCell ref="S490:S491"/>
+    <mergeCell ref="R490:R491"/>
+    <mergeCell ref="O490:O491"/>
+    <mergeCell ref="N490:N491"/>
+    <mergeCell ref="P490:P491"/>
+    <mergeCell ref="Q490:Q491"/>
     <mergeCell ref="D490:D491"/>
     <mergeCell ref="C490:C491"/>
     <mergeCell ref="B490:B491"/>
@@ -45196,15 +45212,6 @@
     <mergeCell ref="G490:G491"/>
     <mergeCell ref="F490:F491"/>
     <mergeCell ref="E490:E491"/>
-    <mergeCell ref="M490:M491"/>
-    <mergeCell ref="L490:L491"/>
-    <mergeCell ref="K490:K491"/>
-    <mergeCell ref="S490:S491"/>
-    <mergeCell ref="R490:R491"/>
-    <mergeCell ref="O490:O491"/>
-    <mergeCell ref="N490:N491"/>
-    <mergeCell ref="P490:P491"/>
-    <mergeCell ref="Q490:Q491"/>
   </mergeCells>
   <conditionalFormatting sqref="L492:M1048576 S492:S1048576 AB411 L391:M410 L412:M441 S412:S441 S298 L294:M294 L294:L298 M308 S296 S390:S394 L197:M292 L191:M195 L165:M189 AC164 L3:M137 L139:M163 S1:S163 S165:S189 M442:M445 S191:S294 L300:L311 S396:S410">
     <cfRule type="cellIs" dxfId="7" priority="30" operator="greaterThan">
@@ -45274,6 +45281,11 @@
     <hyperlink ref="W355" r:id="rId25"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId26"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>